<commit_message>
Updating node splitting algorithm
</commit_message>
<xml_diff>
--- a/Tables/Word_similarity_summary_combined_clics3based_SimVerb.xlsx
+++ b/Tables/Word_similarity_summary_combined_clics3based_SimVerb.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Network</t>
   </si>
@@ -63,12 +63,6 @@
   </si>
   <si>
     <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
   </si>
   <si>
     <t>combined</t>
@@ -184,16 +178,16 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D2" t="n">
         <v>1719.0</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F2" t="n">
         <v>794.0</v>
@@ -230,112 +224,6 @@
       </c>
       <c r="Q2" t="n">
         <v>8.718616529714635E-68</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="M3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="N3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="O3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="P3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="Q3" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="M4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="N4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="O4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="P4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="Q4" t="e">
-        <v>#N/A</v>
       </c>
     </row>
   </sheetData>

</xml_diff>